<commit_message>
removed AV131 from processed meat in DPE_KORA_S1_P1 and DPE_KORA_S1_P2
removed DV131 from processed meat in DPE_KORA_S3_P1 and DPE_KORA_S3_P2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09E65193-6A75-41B6-BC12-170035029E7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{ADA90379-EBE1-4BC2-986F-62C8A6EFEA29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -910,15 +899,6 @@
     <t>Intake of processed or preserved meat [g/d]</t>
   </si>
   <si>
-    <t>AV131; AV141; AV145; AV147; AV150; AV160</t>
-  </si>
-  <si>
-    <t>AV131 + AV141 + AV145 + AV147 + AV150 + AV160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV131 (all kinds of minced meat) + AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
-  </si>
-  <si>
     <t>OFFALS_0705</t>
   </si>
   <si>
@@ -1503,6 +1483,15 @@
   </si>
   <si>
     <t>intake of amphibians, reptiles, snails, insects [g/d]</t>
+  </si>
+  <si>
+    <t>AV141; AV145; AV147; AV150; AV160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
+  </si>
+  <si>
+    <t>AV141 + AV145 + AV147 + AV150 + AV160</t>
   </si>
 </sst>
 </file>
@@ -2544,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4798,16 +4787,16 @@
         <v>14</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>251</v>
+        <v>443</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>252</v>
+        <v>445</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>253</v>
+        <v>444</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>57</v>
@@ -4821,10 +4810,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D67" s="20" t="s">
         <v>32</v>
@@ -4833,7 +4822,7 @@
         <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>23</v>
@@ -4842,7 +4831,7 @@
         <v>23</v>
       </c>
       <c r="I67" s="31" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>57</v>
@@ -4856,10 +4845,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D68" s="20" t="s">
         <v>32</v>
@@ -4868,16 +4857,16 @@
         <v>14</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>57</v>
@@ -4891,10 +4880,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>32</v>
@@ -4903,7 +4892,7 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>23</v>
@@ -4912,7 +4901,7 @@
         <v>23</v>
       </c>
       <c r="I69" s="31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>57</v>
@@ -4926,10 +4915,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D70" s="20" t="s">
         <v>32</v>
@@ -4959,10 +4948,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>32</v>
@@ -4971,16 +4960,16 @@
         <v>14</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I71" s="32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>57</v>
@@ -4994,10 +4983,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>32</v>
@@ -5006,16 +4995,16 @@
         <v>14</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I72" s="31" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>57</v>
@@ -5029,10 +5018,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>32</v>
@@ -5041,7 +5030,7 @@
         <v>14</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>23</v>
@@ -5050,7 +5039,7 @@
         <v>23</v>
       </c>
       <c r="I73" s="31" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>57</v>
@@ -5064,10 +5053,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>32</v>
@@ -5076,16 +5065,16 @@
         <v>14</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I74" s="32" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>57</v>
@@ -5099,10 +5088,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>32</v>
@@ -5111,7 +5100,7 @@
         <v>14</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>23</v>
@@ -5120,7 +5109,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="31" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>57</v>
@@ -5134,10 +5123,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>32</v>
@@ -5146,7 +5135,7 @@
         <v>14</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>23</v>
@@ -5155,7 +5144,7 @@
         <v>23</v>
       </c>
       <c r="I76" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>57</v>
@@ -5169,10 +5158,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>32</v>
@@ -5181,7 +5170,7 @@
         <v>14</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>23</v>
@@ -5190,7 +5179,7 @@
         <v>23</v>
       </c>
       <c r="I77" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>57</v>
@@ -5204,10 +5193,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C78" s="45" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>32</v>
@@ -5237,10 +5226,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>32</v>
@@ -5269,10 +5258,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>32</v>
@@ -5301,10 +5290,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D81" s="20" t="s">
         <v>32</v>
@@ -5313,16 +5302,16 @@
         <v>14</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I81" s="32" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>57</v>
@@ -5336,10 +5325,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C82" s="45" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>32</v>
@@ -5348,16 +5337,16 @@
         <v>14</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I82" s="31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>57</v>
@@ -5371,10 +5360,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D83" s="20" t="s">
         <v>32</v>
@@ -5383,16 +5372,16 @@
         <v>14</v>
       </c>
       <c r="F83" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H83" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I83" s="32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>57</v>
@@ -5406,10 +5395,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C84" s="45" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D84" s="20" t="s">
         <v>32</v>
@@ -5418,7 +5407,7 @@
         <v>14</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>23</v>
@@ -5427,7 +5416,7 @@
         <v>23</v>
       </c>
       <c r="I84" s="20" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>57</v>
@@ -5441,10 +5430,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>32</v>
@@ -5474,10 +5463,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C86" s="45" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D86" s="20" t="s">
         <v>32</v>
@@ -5506,10 +5495,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D87" s="20" t="s">
         <v>32</v>
@@ -5518,7 +5507,7 @@
         <v>14</v>
       </c>
       <c r="F87" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G87" s="3" t="s">
         <v>23</v>
@@ -5527,7 +5516,7 @@
         <v>23</v>
       </c>
       <c r="I87" s="25" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>57</v>
@@ -5541,10 +5530,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C88" s="45" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D88" s="20" t="s">
         <v>32</v>
@@ -5574,10 +5563,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C89" s="45" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D89" s="20" t="s">
         <v>32</v>
@@ -5607,10 +5596,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C90" s="45" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>32</v>
@@ -5619,16 +5608,16 @@
         <v>14</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>49</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I90" s="33" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>57</v>
@@ -5642,10 +5631,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C91" s="45" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D91" s="20" t="s">
         <v>32</v>
@@ -5675,10 +5664,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D92" s="20" t="s">
         <v>32</v>
@@ -5708,10 +5697,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D93" s="20" t="s">
         <v>32</v>
@@ -5720,16 +5709,16 @@
         <v>14</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I93" s="34" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>57</v>
@@ -5743,10 +5732,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D94" s="20" t="s">
         <v>32</v>
@@ -5755,7 +5744,7 @@
         <v>14</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>23</v>
@@ -5764,7 +5753,7 @@
         <v>23</v>
       </c>
       <c r="I94" s="31" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>57</v>
@@ -5778,10 +5767,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>32</v>
@@ -5790,16 +5779,16 @@
         <v>14</v>
       </c>
       <c r="F95" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H95" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="I95" s="24" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>57</v>
@@ -5813,10 +5802,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D96" s="20" t="s">
         <v>32</v>
@@ -5825,16 +5814,16 @@
         <v>14</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I96" s="32" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>57</v>
@@ -5848,10 +5837,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D97" s="20" t="s">
         <v>32</v>
@@ -5860,16 +5849,16 @@
         <v>14</v>
       </c>
       <c r="F97" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H97" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>57</v>
@@ -5883,10 +5872,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C98" s="45" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D98" s="20" t="s">
         <v>32</v>
@@ -5895,7 +5884,7 @@
         <v>14</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>23</v>
@@ -5904,7 +5893,7 @@
         <v>23</v>
       </c>
       <c r="I98" s="31" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>57</v>
@@ -5918,10 +5907,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C99" s="45" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>32</v>
@@ -5950,10 +5939,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C100" s="45" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D100" s="20" t="s">
         <v>32</v>
@@ -5983,10 +5972,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C101" s="45" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D101" s="20" t="s">
         <v>32</v>
@@ -5995,7 +5984,7 @@
         <v>14</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>23</v>
@@ -6004,7 +5993,7 @@
         <v>23</v>
       </c>
       <c r="I101" s="31" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>57</v>
@@ -6018,10 +6007,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C102" s="45" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D102" s="20" t="s">
         <v>32</v>
@@ -6030,16 +6019,16 @@
         <v>14</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="I102" s="34" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>57</v>
@@ -6053,10 +6042,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C103" s="45" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D103" s="20" t="s">
         <v>32</v>
@@ -6065,16 +6054,16 @@
         <v>14</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I103" s="34" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>57</v>
@@ -6088,10 +6077,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C104" s="45" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D104" s="20" t="s">
         <v>32</v>
@@ -6121,10 +6110,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C105" s="45" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D105" s="20" t="s">
         <v>32</v>
@@ -6133,7 +6122,7 @@
         <v>14</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>23</v>
@@ -6142,7 +6131,7 @@
         <v>23</v>
       </c>
       <c r="I105" s="20" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>57</v>
@@ -6156,10 +6145,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C106" s="45" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D106" s="20" t="s">
         <v>32</v>
@@ -6168,7 +6157,7 @@
         <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>23</v>
@@ -6177,7 +6166,7 @@
         <v>23</v>
       </c>
       <c r="I106" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>57</v>
@@ -6191,10 +6180,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C107" s="45" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D107" s="20" t="s">
         <v>32</v>
@@ -6223,10 +6212,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C108" s="45" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D108" s="20" t="s">
         <v>32</v>
@@ -6255,10 +6244,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C109" s="45" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D109" s="20" t="s">
         <v>32</v>
@@ -6287,10 +6276,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C110" s="45" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D110" s="20" t="s">
         <v>32</v>
@@ -6319,10 +6308,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C111" s="45" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D111" s="20" t="s">
         <v>32</v>
@@ -6352,10 +6341,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C112" s="45" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D112" s="20" t="s">
         <v>32</v>
@@ -6385,10 +6374,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C113" s="45" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D113" s="20" t="s">
         <v>32</v>
@@ -6418,10 +6407,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C114" s="45" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D114" s="20" t="s">
         <v>32</v>
@@ -6451,10 +6440,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C115" s="45" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D115" s="20" t="s">
         <v>32</v>
@@ -6484,10 +6473,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C116" s="45" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D116" s="20" t="s">
         <v>32</v>
@@ -6517,10 +6506,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C117" s="45" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D117" s="20" t="s">
         <v>32</v>
@@ -6550,10 +6539,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C118" s="45" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D118" s="20" t="s">
         <v>32</v>
@@ -6583,10 +6572,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C119" s="45" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D119" s="20" t="s">
         <v>32</v>
@@ -6615,10 +6604,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C120" s="45" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D120" s="20" t="s">
         <v>32</v>
@@ -6647,10 +6636,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C121" s="45" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D121" s="20" t="s">
         <v>32</v>
@@ -6679,10 +6668,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C122" s="45" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D122" s="20" t="s">
         <v>32</v>
@@ -6711,10 +6700,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C123" s="45" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D123" s="20" t="s">
         <v>32</v>
@@ -6743,10 +6732,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C124" s="45" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D124" s="20" t="s">
         <v>32</v>
@@ -6775,10 +6764,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C125" s="45" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D125" s="20" t="s">
         <v>32</v>
@@ -6807,10 +6796,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C126" s="45" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D126" s="20" t="s">
         <v>32</v>
@@ -6839,10 +6828,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C127" s="45" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D127" s="20" t="s">
         <v>32</v>
@@ -6871,10 +6860,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C128" s="45" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D128" s="20" t="s">
         <v>32</v>
@@ -6908,6 +6897,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -7148,28 +7158,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7186,29 +7200,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to AV131 and DV131: removed from processed meat in all 4 KORA DPEs
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE936C6-E84B-4F94-A08F-E774A7F468BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E22C67-DA8B-4F63-98AA-2C28A60EBE83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -846,15 +846,6 @@
     <t>Intake of processed or preserved meat [g/d]</t>
   </si>
   <si>
-    <t>AV131; AV141; AV145; AV147; AV150; AV160</t>
-  </si>
-  <si>
-    <t>AV131 + AV141 + AV145 + AV147 + AV150 + AV160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV131 (all kinds of minced meat) + AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
-  </si>
-  <si>
     <t>OFFALS_0705</t>
   </si>
   <si>
@@ -1452,6 +1443,15 @@
   </si>
   <si>
     <t>A_ID</t>
+  </si>
+  <si>
+    <t>AV141; AV145; AV147; AV150; AV160</t>
+  </si>
+  <si>
+    <t>AV141 + AV145 + AV147 + AV150 + AV160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
   </si>
 </sst>
 </file>
@@ -2458,27 +2458,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="19"/>
+    <col min="1" max="1" width="11.44140625" style="19"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="19"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="19"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2513,12 +2513,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>11</v>
@@ -2530,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>13</v>
@@ -2546,7 +2546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J10" s="42" t="s">
         <v>47</v>
@@ -2812,7 +2812,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>64</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>47</v>
@@ -2950,7 +2950,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>64</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J21" s="42" t="s">
         <v>47</v>
@@ -3190,7 +3190,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="285" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>42</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>43</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>44</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>46</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>47</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>49</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>50</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>51</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>53</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>55</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>57</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -4713,16 +4713,16 @@
         <v>12</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>245</v>
+        <v>441</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>246</v>
+        <v>442</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>247</v>
+        <v>443</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>52</v>
@@ -4731,15 +4731,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C67" s="39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>29</v>
@@ -4748,7 +4748,7 @@
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>20</v>
@@ -4757,7 +4757,7 @@
         <v>20</v>
       </c>
       <c r="I67" s="30" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>52</v>
@@ -4766,15 +4766,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C68" s="39" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>29</v>
@@ -4783,16 +4783,16 @@
         <v>12</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>52</v>
@@ -4801,15 +4801,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C69" s="39" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>29</v>
@@ -4818,7 +4818,7 @@
         <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>20</v>
@@ -4827,7 +4827,7 @@
         <v>20</v>
       </c>
       <c r="I69" s="30" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>52</v>
@@ -4836,15 +4836,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>29</v>
@@ -4869,15 +4869,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>29</v>
@@ -4886,16 +4886,16 @@
         <v>12</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I71" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>52</v>
@@ -4904,15 +4904,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C72" s="39" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>29</v>
@@ -4921,16 +4921,16 @@
         <v>12</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I72" s="30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>52</v>
@@ -4939,15 +4939,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C73" s="39" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>29</v>
@@ -4956,7 +4956,7 @@
         <v>12</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>20</v>
@@ -4965,7 +4965,7 @@
         <v>20</v>
       </c>
       <c r="I73" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>52</v>
@@ -4974,15 +4974,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>29</v>
@@ -4991,16 +4991,16 @@
         <v>12</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I74" s="31" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>52</v>
@@ -5009,15 +5009,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D75" s="19" t="s">
         <v>29</v>
@@ -5026,7 +5026,7 @@
         <v>12</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>20</v>
@@ -5035,7 +5035,7 @@
         <v>20</v>
       </c>
       <c r="I75" s="30" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>52</v>
@@ -5044,15 +5044,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="19">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>29</v>
@@ -5061,7 +5061,7 @@
         <v>12</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>20</v>
@@ -5070,7 +5070,7 @@
         <v>20</v>
       </c>
       <c r="I76" s="30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>52</v>
@@ -5079,15 +5079,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C77" s="39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D77" s="19" t="s">
         <v>29</v>
@@ -5096,7 +5096,7 @@
         <v>12</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>20</v>
@@ -5105,7 +5105,7 @@
         <v>20</v>
       </c>
       <c r="I77" s="30" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>52</v>
@@ -5114,15 +5114,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C78" s="39" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D78" s="19" t="s">
         <v>29</v>
@@ -5147,15 +5147,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C79" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>29</v>
@@ -5179,15 +5179,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C80" s="39" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D80" s="19" t="s">
         <v>29</v>
@@ -5211,15 +5211,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C81" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>29</v>
@@ -5228,16 +5228,16 @@
         <v>12</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I81" s="31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>52</v>
@@ -5246,15 +5246,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C82" s="39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D82" s="19" t="s">
         <v>29</v>
@@ -5263,16 +5263,16 @@
         <v>12</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I82" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>52</v>
@@ -5281,15 +5281,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C83" s="39" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D83" s="19" t="s">
         <v>29</v>
@@ -5298,16 +5298,16 @@
         <v>12</v>
       </c>
       <c r="F83" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H83" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I83" s="31" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>52</v>
@@ -5316,15 +5316,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C84" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D84" s="19" t="s">
         <v>29</v>
@@ -5333,7 +5333,7 @@
         <v>12</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>20</v>
@@ -5342,7 +5342,7 @@
         <v>20</v>
       </c>
       <c r="I84" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>52</v>
@@ -5351,15 +5351,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C85" s="39" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D85" s="19" t="s">
         <v>29</v>
@@ -5384,15 +5384,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C86" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>29</v>
@@ -5416,15 +5416,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>29</v>
@@ -5433,7 +5433,7 @@
         <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G87" s="3" t="s">
         <v>20</v>
@@ -5442,7 +5442,7 @@
         <v>20</v>
       </c>
       <c r="I87" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>52</v>
@@ -5451,15 +5451,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C88" s="39" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D88" s="19" t="s">
         <v>29</v>
@@ -5484,15 +5484,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C89" s="39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D89" s="19" t="s">
         <v>29</v>
@@ -5517,15 +5517,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C90" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D90" s="19" t="s">
         <v>29</v>
@@ -5534,16 +5534,16 @@
         <v>12</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>45</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I90" s="32" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>52</v>
@@ -5552,15 +5552,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C91" s="39" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D91" s="19" t="s">
         <v>29</v>
@@ -5585,15 +5585,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C92" s="39" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D92" s="19" t="s">
         <v>29</v>
@@ -5618,15 +5618,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D93" s="19" t="s">
         <v>29</v>
@@ -5635,16 +5635,16 @@
         <v>12</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I93" s="33" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>52</v>
@@ -5653,15 +5653,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D94" s="19" t="s">
         <v>29</v>
@@ -5670,7 +5670,7 @@
         <v>12</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>20</v>
@@ -5679,7 +5679,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>52</v>
@@ -5688,15 +5688,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C95" s="39" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>29</v>
@@ -5705,16 +5705,16 @@
         <v>12</v>
       </c>
       <c r="F95" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H95" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>52</v>
@@ -5723,15 +5723,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="19">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C96" s="39" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D96" s="19" t="s">
         <v>29</v>
@@ -5740,16 +5740,16 @@
         <v>12</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I96" s="31" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>52</v>
@@ -5758,15 +5758,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C97" s="39" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D97" s="19" t="s">
         <v>29</v>
@@ -5775,16 +5775,16 @@
         <v>12</v>
       </c>
       <c r="F97" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H97" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I97" s="31" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>52</v>
@@ -5793,15 +5793,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C98" s="39" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>29</v>
@@ -5810,7 +5810,7 @@
         <v>12</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>20</v>
@@ -5819,7 +5819,7 @@
         <v>20</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>52</v>
@@ -5828,15 +5828,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C99" s="39" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>29</v>
@@ -5860,15 +5860,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C100" s="39" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D100" s="19" t="s">
         <v>29</v>
@@ -5893,15 +5893,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C101" s="39" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D101" s="19" t="s">
         <v>29</v>
@@ -5910,7 +5910,7 @@
         <v>12</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>20</v>
@@ -5919,7 +5919,7 @@
         <v>20</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>52</v>
@@ -5928,15 +5928,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C102" s="39" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D102" s="19" t="s">
         <v>29</v>
@@ -5945,16 +5945,16 @@
         <v>12</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I102" s="33" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>52</v>
@@ -5963,15 +5963,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C103" s="39" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D103" s="19" t="s">
         <v>29</v>
@@ -5980,16 +5980,16 @@
         <v>12</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I103" s="33" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>52</v>
@@ -5998,15 +5998,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C104" s="39" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D104" s="19" t="s">
         <v>29</v>
@@ -6031,15 +6031,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="19">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C105" s="39" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D105" s="19" t="s">
         <v>29</v>
@@ -6048,7 +6048,7 @@
         <v>12</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>20</v>
@@ -6057,7 +6057,7 @@
         <v>20</v>
       </c>
       <c r="I105" s="19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>52</v>
@@ -6066,15 +6066,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C106" s="39" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D106" s="19" t="s">
         <v>29</v>
@@ -6083,7 +6083,7 @@
         <v>12</v>
       </c>
       <c r="F106" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>20</v>
@@ -6092,7 +6092,7 @@
         <v>20</v>
       </c>
       <c r="I106" s="19" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>52</v>
@@ -6101,15 +6101,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C107" s="39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D107" s="19" t="s">
         <v>29</v>
@@ -6133,15 +6133,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A108" s="19">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C108" s="39" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D108" s="19" t="s">
         <v>29</v>
@@ -6165,15 +6165,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="19">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C109" s="39" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D109" s="19" t="s">
         <v>29</v>
@@ -6197,15 +6197,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="19">
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C110" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D110" s="19" t="s">
         <v>29</v>
@@ -6229,15 +6229,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="19">
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C111" s="39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D111" s="19" t="s">
         <v>29</v>
@@ -6262,15 +6262,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="19">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C112" s="39" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D112" s="19" t="s">
         <v>29</v>
@@ -6295,15 +6295,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="19">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>29</v>
@@ -6328,15 +6328,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>29</v>
@@ -6361,15 +6361,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="19">
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D115" s="19" t="s">
         <v>29</v>
@@ -6394,15 +6394,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="19">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C116" s="39" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>29</v>
@@ -6427,15 +6427,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="19">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C117" s="39" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>29</v>
@@ -6460,15 +6460,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="19">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C118" s="39" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>29</v>
@@ -6493,15 +6493,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="19">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C119" s="39" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D119" s="19" t="s">
         <v>29</v>
@@ -6525,15 +6525,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="19">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C120" s="39" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D120" s="19" t="s">
         <v>29</v>
@@ -6557,15 +6557,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="19">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C121" s="39" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D121" s="19" t="s">
         <v>29</v>
@@ -6589,15 +6589,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122" s="19">
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C122" s="39" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D122" s="19" t="s">
         <v>29</v>
@@ -6621,15 +6621,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="19">
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C123" s="39" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D123" s="19" t="s">
         <v>29</v>
@@ -6653,15 +6653,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124" s="19">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C124" s="39" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D124" s="19" t="s">
         <v>29</v>
@@ -6685,15 +6685,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="19">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C125" s="39" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D125" s="19" t="s">
         <v>29</v>
@@ -6717,15 +6717,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="19">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C126" s="39" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D126" s="19" t="s">
         <v>29</v>
@@ -6749,15 +6749,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="19">
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C127" s="39" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D127" s="19" t="s">
         <v>29</v>
@@ -6781,15 +6781,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="19">
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C128" s="39" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D128" s="19" t="s">
         <v>29</v>
@@ -6835,15 +6835,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -7084,6 +7075,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
   <ds:schemaRefs>
@@ -7102,14 +7102,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7126,4 +7118,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed the id variable name to a_id
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E22C67-DA8B-4F63-98AA-2C28A60EBE83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5E945E52-AEAD-4EC1-8112-4383EF12C635}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -1442,9 +1442,6 @@
     <t>AV440 (leafy and stem vegetables) Gewichtung mit 0,5 sinnvoll?</t>
   </si>
   <si>
-    <t>A_ID</t>
-  </si>
-  <si>
     <t>AV141; AV145; AV147; AV150; AV160</t>
   </si>
   <si>
@@ -1452,6 +1449,9 @@
   </si>
   <si>
     <t xml:space="preserve">AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
+  </si>
+  <si>
+    <t>a_id</t>
   </si>
 </sst>
 </file>
@@ -2458,27 +2458,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="19"/>
+    <col min="1" max="1" width="11.42578125" style="19"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="19"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="19"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>13</v>
@@ -2546,7 +2546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="285" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>42</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>43</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>44</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>46</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>47</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="19">
         <v>49</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
         <v>50</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="19">
         <v>51</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
         <v>53</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="19">
         <v>55</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>57</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -4713,16 +4713,16 @@
         <v>12</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H66" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="I66" s="23" t="s">
         <v>442</v>
-      </c>
-      <c r="I66" s="23" t="s">
-        <v>443</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>52</v>
@@ -4731,7 +4731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="19">
         <v>71</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="19">
         <v>74</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="19">
         <v>75</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19">
         <v>76</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="19">
         <v>77</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="19">
         <v>78</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="19">
         <v>79</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="19">
         <v>80</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="19">
         <v>81</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="19">
         <v>82</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="19">
         <v>83</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="19">
         <v>84</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="19">
         <v>85</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="19">
         <v>86</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19">
         <v>87</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="19">
         <v>88</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="19">
         <v>89</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="19">
         <v>90</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="19">
         <v>91</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="19">
         <v>92</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="19">
         <v>93</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="19">
         <v>94</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="19">
         <v>95</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="19">
         <v>96</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="19">
         <v>97</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="19">
         <v>98</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="19">
         <v>99</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="19">
         <v>100</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="19">
         <v>101</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="19">
         <v>102</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="19">
         <v>103</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="19">
         <v>104</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="19">
         <v>105</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="19">
         <v>106</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="19">
         <v>107</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="19">
         <v>108</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" s="19">
         <v>109</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="19">
         <v>110</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="19">
         <v>111</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="19">
         <v>112</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="19">
         <v>113</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="19">
         <v>114</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="19">
         <v>115</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="19">
         <v>116</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="19">
         <v>117</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="19">
         <v>118</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="19">
         <v>119</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="19">
         <v>120</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="19">
         <v>121</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="19">
         <v>122</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="19">
         <v>123</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="19">
         <v>124</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="19">
         <v>125</v>
       </c>
@@ -6749,7 +6749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="19">
         <v>126</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="19">
         <v>127</v>
       </c>
@@ -6823,15 +6823,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7076,27 +7073,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7121,9 +7112,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding paste operation on dietary assessment instrument
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5E945E52-AEAD-4EC1-8112-4383EF12C635}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC078A85-A0D9-44EE-BD14-9B9B5CE81389}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="449">
   <si>
     <t>index</t>
   </si>
@@ -1453,12 +1453,27 @@
   <si>
     <t>a_id</t>
   </si>
+  <si>
+    <t>DIETARY_ASSESS_INSTR</t>
+  </si>
+  <si>
+    <t>Dietary Assessment Instrument</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
+  </si>
+  <si>
+    <t>paste</t>
+  </si>
+  <si>
+    <t>5 (7_d_FR_w)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1645,6 +1660,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1995,7 +2016,7 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2100,6 +2121,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2456,29 +2478,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L128"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="19"/>
+    <col min="1" max="1" width="11.44140625" style="19"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="19"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="19"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -2546,7 +2568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -2579,7 +2601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -2612,7 +2634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2645,7 +2667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2678,7 +2700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -2711,7 +2733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2744,7 +2766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2777,7 +2799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2812,7 +2834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2847,7 +2869,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2880,7 +2902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2915,7 +2937,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2950,7 +2972,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -2985,7 +3007,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3020,7 +3042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3055,7 +3077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3087,7 +3109,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3120,7 +3142,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3155,7 +3177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3190,7 +3212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -3223,7 +3245,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -3258,7 +3280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -3291,7 +3313,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="285" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -3326,7 +3348,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -3361,7 +3383,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -3396,7 +3418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -3431,7 +3453,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -3464,7 +3486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -3499,7 +3521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -3534,7 +3556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -3567,7 +3589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -3602,7 +3624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -3637,7 +3659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -3672,7 +3694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -3704,7 +3726,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -3737,7 +3759,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -3772,7 +3794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -3805,7 +3827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -3840,7 +3862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -3875,7 +3897,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -3910,7 +3932,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>42</v>
       </c>
@@ -3945,7 +3967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>43</v>
       </c>
@@ -3981,7 +4003,7 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>44</v>
       </c>
@@ -4016,7 +4038,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -4051,7 +4073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>46</v>
       </c>
@@ -4083,7 +4105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>47</v>
       </c>
@@ -4115,7 +4137,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -4150,7 +4172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>49</v>
       </c>
@@ -4185,7 +4207,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>50</v>
       </c>
@@ -4220,7 +4242,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>51</v>
       </c>
@@ -4255,7 +4277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -4290,7 +4312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>53</v>
       </c>
@@ -4325,7 +4347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -4360,7 +4382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>55</v>
       </c>
@@ -4393,7 +4415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -4428,7 +4450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>57</v>
       </c>
@@ -4463,7 +4485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -4496,7 +4518,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -4529,7 +4551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -4562,7 +4584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -4595,7 +4617,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -4628,7 +4650,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -4661,7 +4683,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -4696,7 +4718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -4731,7 +4753,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -4766,7 +4788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -4801,7 +4823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -4836,7 +4858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -4869,7 +4891,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -4904,7 +4926,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>71</v>
       </c>
@@ -4939,7 +4961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -4974,7 +4996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -5009,7 +5031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <v>74</v>
       </c>
@@ -5044,7 +5066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="19">
         <v>75</v>
       </c>
@@ -5079,7 +5101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>76</v>
       </c>
@@ -5114,7 +5136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>77</v>
       </c>
@@ -5147,7 +5169,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>78</v>
       </c>
@@ -5179,7 +5201,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>79</v>
       </c>
@@ -5211,7 +5233,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>80</v>
       </c>
@@ -5246,7 +5268,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>81</v>
       </c>
@@ -5281,7 +5303,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>82</v>
       </c>
@@ -5316,7 +5338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>83</v>
       </c>
@@ -5351,7 +5373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>84</v>
       </c>
@@ -5384,7 +5406,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>85</v>
       </c>
@@ -5416,7 +5438,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>86</v>
       </c>
@@ -5451,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>87</v>
       </c>
@@ -5484,7 +5506,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <v>88</v>
       </c>
@@ -5517,7 +5539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>89</v>
       </c>
@@ -5552,7 +5574,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>90</v>
       </c>
@@ -5585,7 +5607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>91</v>
       </c>
@@ -5618,7 +5640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>92</v>
       </c>
@@ -5653,7 +5675,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>93</v>
       </c>
@@ -5688,7 +5710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>94</v>
       </c>
@@ -5723,7 +5745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="19">
         <v>95</v>
       </c>
@@ -5758,7 +5780,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>96</v>
       </c>
@@ -5793,7 +5815,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>97</v>
       </c>
@@ -5828,7 +5850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>98</v>
       </c>
@@ -5860,7 +5882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>99</v>
       </c>
@@ -5893,7 +5915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>100</v>
       </c>
@@ -5928,7 +5950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>101</v>
       </c>
@@ -5963,7 +5985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <v>102</v>
       </c>
@@ -5998,7 +6020,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>103</v>
       </c>
@@ -6031,7 +6053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="19">
         <v>104</v>
       </c>
@@ -6066,7 +6088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>105</v>
       </c>
@@ -6101,7 +6123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
         <v>106</v>
       </c>
@@ -6133,7 +6155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A108" s="19">
         <v>107</v>
       </c>
@@ -6165,7 +6187,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="19">
         <v>108</v>
       </c>
@@ -6197,7 +6219,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="19">
         <v>109</v>
       </c>
@@ -6229,7 +6251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="19">
         <v>110</v>
       </c>
@@ -6262,7 +6284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="19">
         <v>111</v>
       </c>
@@ -6295,7 +6317,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="19">
         <v>112</v>
       </c>
@@ -6328,7 +6350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>113</v>
       </c>
@@ -6361,7 +6383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="19">
         <v>114</v>
       </c>
@@ -6394,7 +6416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="19">
         <v>115</v>
       </c>
@@ -6427,7 +6449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="19">
         <v>116</v>
       </c>
@@ -6460,7 +6482,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="19">
         <v>117</v>
       </c>
@@ -6493,7 +6515,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="19">
         <v>118</v>
       </c>
@@ -6525,7 +6547,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="19">
         <v>119</v>
       </c>
@@ -6557,7 +6579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="19">
         <v>120</v>
       </c>
@@ -6589,7 +6611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122" s="19">
         <v>121</v>
       </c>
@@ -6621,7 +6643,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="19">
         <v>122</v>
       </c>
@@ -6653,7 +6675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124" s="19">
         <v>123</v>
       </c>
@@ -6685,7 +6707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="19">
         <v>124</v>
       </c>
@@ -6717,7 +6739,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="19">
         <v>125</v>
       </c>
@@ -6749,7 +6771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="19">
         <v>126</v>
       </c>
@@ -6781,7 +6803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="19">
         <v>127</v>
       </c>
@@ -6811,6 +6833,41 @@
       </c>
       <c r="K128" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="19">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>444</v>
+      </c>
+      <c r="C129" t="s">
+        <v>445</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E129" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F129" s="46" t="s">
+        <v>446</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="H129">
+        <v>5</v>
+      </c>
+      <c r="I129" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="J129" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="K129" s="41" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -6819,6 +6876,7 @@
     <hyperlink ref="B7" r:id="rId2" display="https://mica.mdc-berlin.de/variable/microbiome-in-health-and-disease-and-in-ageing:SMOKE_ST:Dataschema" xr:uid="{FAD6DFA0-03A7-4E34-8AF3-9DB2877CE1C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6832,6 +6890,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -7072,18 +7142,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
   <ds:schemaRefs>
@@ -7093,6 +7151,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7109,21 +7184,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- for legumes I changed harmonisation potential to compatible and harmonisation rule to operation with respective algortihm - for EGGS_0901 I changed AV255 into AV250
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF856BAC-0E46-4899-8C93-2FB21D27EF86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07A4D58-25F4-44EC-81D2-3DD5F914F1DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="450">
   <si>
     <t>index</t>
   </si>
@@ -310,9 +310,6 @@
   </si>
   <si>
     <t xml:space="preserve">AV491 </t>
-  </si>
-  <si>
-    <t>AV491 (dry legumes) </t>
   </si>
   <si>
     <t>LEGUMES_0301</t>
@@ -892,12 +889,6 @@
     <t>Intake of eggs [g/d]</t>
   </si>
   <si>
-    <t>AV255</t>
-  </si>
-  <si>
-    <t>AV255 (egg products)</t>
-  </si>
-  <si>
     <t>FAT_10</t>
   </si>
   <si>
@@ -1464,6 +1455,18 @@
   </si>
   <si>
     <t>Intake of amphibians, reptiles, snails, insects [g/d]</t>
+  </si>
+  <si>
+    <t>AV491*2</t>
+  </si>
+  <si>
+    <t>double the amount of AV491 (dry legumes) to be comparable to other studies</t>
+  </si>
+  <si>
+    <t>AV250</t>
+  </si>
+  <si>
+    <t>AV250 (fresh eggs)</t>
   </si>
 </sst>
 </file>
@@ -2477,27 +2480,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="19"/>
+    <col min="1" max="1" width="11.42578125" style="19"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="19"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="19"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2532,15 +2535,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D2" s="43" t="s">
         <v>17</v>
@@ -2549,7 +2552,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>12</v>
@@ -2565,7 +2568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -2631,7 +2634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2664,7 +2667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>28</v>
@@ -2763,7 +2766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2796,7 +2799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="J10" s="42" t="s">
         <v>45</v>
@@ -2831,7 +2834,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>62</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>45</v>
@@ -2969,7 +2972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3139,7 +3142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>62</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J21" s="42" t="s">
         <v>45</v>
@@ -3209,7 +3212,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -3262,30 +3265,30 @@
         <v>91</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>92</v>
+        <v>447</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>50</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="39" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>94</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>28</v>
@@ -3310,33 +3313,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="285" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="36" t="s">
         <v>96</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>97</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="23" t="s">
         <v>98</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>99</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>50</v>
@@ -3345,33 +3348,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="D26" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>102</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H26" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="28" t="s">
         <v>103</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>104</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>50</v>
@@ -3380,24 +3383,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="D27" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
         <v>106</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>107</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>19</v>
@@ -3406,7 +3409,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>50</v>
@@ -3415,33 +3418,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="D28" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H28" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="29" t="s">
         <v>112</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>113</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>50</v>
@@ -3450,15 +3453,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="39" t="s">
         <v>114</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>115</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>28</v>
@@ -3483,33 +3486,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="D30" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H30" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="31" t="s">
         <v>119</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>120</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>50</v>
@@ -3518,24 +3521,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="D31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>19</v>
@@ -3544,7 +3547,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>50</v>
@@ -3553,15 +3556,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="39" t="s">
         <v>125</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>126</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>28</v>
@@ -3586,24 +3589,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="D33" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
         <v>128</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>129</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>19</v>
@@ -3612,7 +3615,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>50</v>
@@ -3621,24 +3624,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="D34" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="37" t="s">
         <v>132</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="37" t="s">
-        <v>133</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>19</v>
@@ -3647,7 +3650,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>50</v>
@@ -3656,24 +3659,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>432</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
         <v>135</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>435</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>136</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>19</v>
@@ -3682,7 +3685,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>50</v>
@@ -3691,15 +3694,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>28</v>
@@ -3723,15 +3726,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="39" t="s">
         <v>139</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>140</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>28</v>
@@ -3756,24 +3759,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="D38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>142</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>143</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>19</v>
@@ -3782,7 +3785,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>50</v>
@@ -3791,15 +3794,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>28</v>
@@ -3824,24 +3827,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="D40" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
         <v>147</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" t="s">
-        <v>148</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>19</v>
@@ -3850,7 +3853,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>50</v>
@@ -3859,33 +3862,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>435</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>438</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H41" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="31" t="s">
         <v>152</v>
-      </c>
-      <c r="I41" s="31" t="s">
-        <v>153</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>50</v>
@@ -3894,33 +3897,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="D42" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>156</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I42" s="31" t="s">
         <v>157</v>
-      </c>
-      <c r="I42" s="31" t="s">
-        <v>158</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>50</v>
@@ -3929,33 +3932,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="D43" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I43" s="30" t="s">
         <v>162</v>
-      </c>
-      <c r="I43" s="30" t="s">
-        <v>163</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>50</v>
@@ -3964,33 +3967,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="D44" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="36" t="s">
         <v>165</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>166</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H44" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="I44" s="32" t="s">
         <v>167</v>
-      </c>
-      <c r="I44" s="32" t="s">
-        <v>168</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>50</v>
@@ -4000,33 +4003,33 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="D45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H45" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I45" s="32" t="s">
         <v>172</v>
-      </c>
-      <c r="I45" s="32" t="s">
-        <v>173</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>50</v>
@@ -4035,24 +4038,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="D46" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="37" t="s">
         <v>175</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="37" t="s">
-        <v>176</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>19</v>
@@ -4061,7 +4064,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>50</v>
@@ -4070,15 +4073,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="39" t="s">
         <v>178</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>179</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>28</v>
@@ -4102,15 +4105,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="39" t="s">
         <v>180</v>
-      </c>
-      <c r="C48" s="39" t="s">
-        <v>181</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>28</v>
@@ -4134,15 +4137,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>28</v>
@@ -4160,7 +4163,7 @@
         <v>30</v>
       </c>
       <c r="I49" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>30</v>
@@ -4169,33 +4172,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="19">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="D50" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H50" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I50" s="23" t="s">
         <v>187</v>
-      </c>
-      <c r="I50" s="23" t="s">
-        <v>188</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>50</v>
@@ -4204,33 +4207,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C51" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="D51" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I51" s="31" t="s">
         <v>192</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>193</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>50</v>
@@ -4239,24 +4242,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="19">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="C52" s="39" t="s">
+      <c r="D52" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>19</v>
@@ -4265,7 +4268,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>50</v>
@@ -4274,24 +4277,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="D53" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>19</v>
@@ -4300,7 +4303,7 @@
         <v>19</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>50</v>
@@ -4309,24 +4312,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="D54" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>19</v>
@@ -4335,7 +4338,7 @@
         <v>19</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>50</v>
@@ -4344,33 +4347,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="D55" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H55" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="I55" s="28" t="s">
         <v>209</v>
-      </c>
-      <c r="I55" s="28" t="s">
-        <v>210</v>
       </c>
       <c r="J55" s="42" t="s">
         <v>45</v>
@@ -4379,15 +4382,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="19">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C56" s="39" t="s">
         <v>211</v>
-      </c>
-      <c r="C56" s="39" t="s">
-        <v>212</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>28</v>
@@ -4412,16 +4415,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C57" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="C57" s="39" t="s">
-        <v>214</v>
-      </c>
       <c r="D57" s="19" t="s">
         <v>28</v>
       </c>
@@ -4429,16 +4432,16 @@
         <v>11</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I57" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J57" s="42" t="s">
         <v>45</v>
@@ -4447,24 +4450,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C58" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="D58" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
         <v>217</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" t="s">
-        <v>218</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>19</v>
@@ -4473,7 +4476,7 @@
         <v>19</v>
       </c>
       <c r="I58" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>50</v>
@@ -4482,15 +4485,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="19">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C59" s="39" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>28</v>
@@ -4515,15 +4518,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="19">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>28</v>
@@ -4548,15 +4551,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="19">
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C61" s="39" t="s">
         <v>222</v>
-      </c>
-      <c r="C61" s="39" t="s">
-        <v>223</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>28</v>
@@ -4581,15 +4584,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="19">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C62" s="39" t="s">
         <v>224</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>225</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>28</v>
@@ -4614,15 +4617,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="19">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C63" s="39" t="s">
         <v>226</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>227</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>28</v>
@@ -4647,15 +4650,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="19">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C64" s="39" t="s">
         <v>228</v>
-      </c>
-      <c r="C64" s="39" t="s">
-        <v>229</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>28</v>
@@ -4680,24 +4683,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="19">
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C65" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="C65" s="39" t="s">
+      <c r="D65" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" t="s">
         <v>231</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" t="s">
-        <v>232</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>19</v>
@@ -4706,7 +4709,7 @@
         <v>19</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>50</v>
@@ -4715,16 +4718,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="19">
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C66" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="C66" s="39" t="s">
-        <v>235</v>
-      </c>
       <c r="D66" s="19" t="s">
         <v>28</v>
       </c>
@@ -4732,16 +4735,16 @@
         <v>11</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>50</v>
@@ -4750,24 +4753,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="19">
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C67" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="C67" s="39" t="s">
+      <c r="D67" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="s">
         <v>237</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" t="s">
-        <v>238</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>19</v>
@@ -4776,7 +4779,7 @@
         <v>19</v>
       </c>
       <c r="I67" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>50</v>
@@ -4785,33 +4788,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="19">
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C68" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="C68" s="39" t="s">
+      <c r="D68" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H68" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="I68" s="23" t="s">
         <v>243</v>
-      </c>
-      <c r="I68" s="23" t="s">
-        <v>244</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>50</v>
@@ -4820,24 +4823,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="19">
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>439</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
         <v>245</v>
-      </c>
-      <c r="C69" s="39" t="s">
-        <v>442</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>246</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>19</v>
@@ -4846,7 +4849,7 @@
         <v>19</v>
       </c>
       <c r="I69" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>50</v>
@@ -4855,15 +4858,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="19">
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" s="39" t="s">
         <v>248</v>
-      </c>
-      <c r="C70" s="39" t="s">
-        <v>249</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>28</v>
@@ -4888,33 +4891,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="19">
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C71" s="39" t="s">
+        <v>440</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="C71" s="39" t="s">
-        <v>443</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>251</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H71" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I71" s="31" t="s">
         <v>252</v>
-      </c>
-      <c r="I71" s="31" t="s">
-        <v>253</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>50</v>
@@ -4923,33 +4926,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="19">
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>253</v>
+      </c>
+      <c r="C72" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="D72" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H72" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="I72" s="30" t="s">
         <v>257</v>
-      </c>
-      <c r="I72" s="30" t="s">
-        <v>258</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>50</v>
@@ -4958,16 +4961,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="19">
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>258</v>
+      </c>
+      <c r="C73" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="C73" s="39" t="s">
-        <v>260</v>
-      </c>
       <c r="D73" s="19" t="s">
         <v>28</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>11</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>261</v>
+        <v>448</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>19</v>
@@ -4984,7 +4987,7 @@
         <v>19</v>
       </c>
       <c r="I73" s="30" t="s">
-        <v>262</v>
+        <v>449</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>50</v>
@@ -4993,15 +4996,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="19">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>28</v>
@@ -5010,16 +5013,16 @@
         <v>11</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I74" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>50</v>
@@ -5028,15 +5031,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="19">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D75" s="19" t="s">
         <v>28</v>
@@ -5045,7 +5048,7 @@
         <v>11</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>19</v>
@@ -5054,7 +5057,7 @@
         <v>19</v>
       </c>
       <c r="I75" s="30" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>50</v>
@@ -5063,15 +5066,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="19">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>28</v>
@@ -5080,7 +5083,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>19</v>
@@ -5089,7 +5092,7 @@
         <v>19</v>
       </c>
       <c r="I76" s="30" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>50</v>
@@ -5098,15 +5101,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C77" s="39" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D77" s="19" t="s">
         <v>28</v>
@@ -5115,7 +5118,7 @@
         <v>11</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>19</v>
@@ -5124,7 +5127,7 @@
         <v>19</v>
       </c>
       <c r="I77" s="30" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>50</v>
@@ -5133,15 +5136,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="19">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C78" s="39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D78" s="19" t="s">
         <v>28</v>
@@ -5166,15 +5169,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="19">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C79" s="39" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>28</v>
@@ -5198,15 +5201,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="19">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C80" s="39" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D80" s="19" t="s">
         <v>28</v>
@@ -5230,15 +5233,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="19">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C81" s="39" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>28</v>
@@ -5247,16 +5250,16 @@
         <v>11</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I81" s="31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>50</v>
@@ -5265,15 +5268,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="19">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C82" s="39" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D82" s="19" t="s">
         <v>28</v>
@@ -5282,16 +5285,16 @@
         <v>11</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I82" s="30" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>50</v>
@@ -5300,15 +5303,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="19">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C83" s="39" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D83" s="19" t="s">
         <v>28</v>
@@ -5317,16 +5320,16 @@
         <v>11</v>
       </c>
       <c r="F83" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H83" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I83" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>50</v>
@@ -5335,15 +5338,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="19">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C84" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D84" s="19" t="s">
         <v>28</v>
@@ -5352,7 +5355,7 @@
         <v>11</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>19</v>
@@ -5361,7 +5364,7 @@
         <v>19</v>
       </c>
       <c r="I84" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>50</v>
@@ -5370,15 +5373,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="19">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C85" s="39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D85" s="19" t="s">
         <v>28</v>
@@ -5403,15 +5406,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="19">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C86" s="39" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>28</v>
@@ -5435,15 +5438,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="19">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>28</v>
@@ -5452,7 +5455,7 @@
         <v>11</v>
       </c>
       <c r="F87" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G87" s="3" t="s">
         <v>19</v>
@@ -5461,7 +5464,7 @@
         <v>19</v>
       </c>
       <c r="I87" s="24" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>50</v>
@@ -5470,15 +5473,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C88" s="39" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D88" s="19" t="s">
         <v>28</v>
@@ -5503,15 +5506,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="19">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C89" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D89" s="19" t="s">
         <v>28</v>
@@ -5536,15 +5539,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="19">
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C90" s="39" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D90" s="19" t="s">
         <v>28</v>
@@ -5553,16 +5556,16 @@
         <v>11</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I90" s="32" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>50</v>
@@ -5571,15 +5574,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="19">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C91" s="39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D91" s="19" t="s">
         <v>28</v>
@@ -5604,15 +5607,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="19">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C92" s="39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D92" s="19" t="s">
         <v>28</v>
@@ -5637,15 +5640,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="19">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D93" s="19" t="s">
         <v>28</v>
@@ -5654,16 +5657,16 @@
         <v>11</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I93" s="33" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>50</v>
@@ -5672,15 +5675,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="19">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D94" s="19" t="s">
         <v>28</v>
@@ -5689,7 +5692,7 @@
         <v>11</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>19</v>
@@ -5698,7 +5701,7 @@
         <v>19</v>
       </c>
       <c r="I94" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>50</v>
@@ -5707,15 +5710,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="19">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C95" s="39" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>28</v>
@@ -5724,16 +5727,16 @@
         <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H95" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>50</v>
@@ -5742,15 +5745,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="19">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C96" s="39" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D96" s="19" t="s">
         <v>28</v>
@@ -5759,16 +5762,16 @@
         <v>11</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I96" s="31" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>50</v>
@@ -5777,15 +5780,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="19">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C97" s="39" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D97" s="19" t="s">
         <v>28</v>
@@ -5794,16 +5797,16 @@
         <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H97" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I97" s="31" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>50</v>
@@ -5812,15 +5815,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="19">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C98" s="39" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>28</v>
@@ -5829,7 +5832,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>19</v>
@@ -5838,7 +5841,7 @@
         <v>19</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>50</v>
@@ -5847,15 +5850,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="19">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C99" s="39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>28</v>
@@ -5879,15 +5882,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="19">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C100" s="39" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D100" s="19" t="s">
         <v>28</v>
@@ -5912,15 +5915,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="19">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C101" s="39" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D101" s="19" t="s">
         <v>28</v>
@@ -5929,7 +5932,7 @@
         <v>11</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>19</v>
@@ -5938,7 +5941,7 @@
         <v>19</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>50</v>
@@ -5947,15 +5950,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="19">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C102" s="39" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D102" s="19" t="s">
         <v>28</v>
@@ -5964,16 +5967,16 @@
         <v>11</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I102" s="33" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>50</v>
@@ -5982,15 +5985,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="19">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C103" s="39" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D103" s="19" t="s">
         <v>28</v>
@@ -5999,16 +6002,16 @@
         <v>11</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="I103" s="33" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>50</v>
@@ -6017,15 +6020,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="19">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C104" s="39" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D104" s="19" t="s">
         <v>28</v>
@@ -6050,15 +6053,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="19">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C105" s="39" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D105" s="19" t="s">
         <v>28</v>
@@ -6067,7 +6070,7 @@
         <v>11</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>19</v>
@@ -6076,7 +6079,7 @@
         <v>19</v>
       </c>
       <c r="I105" s="19" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>50</v>
@@ -6085,15 +6088,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="19">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C106" s="39" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D106" s="19" t="s">
         <v>28</v>
@@ -6102,7 +6105,7 @@
         <v>11</v>
       </c>
       <c r="F106" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>19</v>
@@ -6111,7 +6114,7 @@
         <v>19</v>
       </c>
       <c r="I106" s="19" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>50</v>
@@ -6120,15 +6123,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="19">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C107" s="39" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D107" s="19" t="s">
         <v>28</v>
@@ -6152,15 +6155,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="19">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C108" s="39" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D108" s="19" t="s">
         <v>28</v>
@@ -6184,15 +6187,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="19">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C109" s="39" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D109" s="19" t="s">
         <v>28</v>
@@ -6216,15 +6219,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" s="19">
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C110" s="39" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D110" s="19" t="s">
         <v>28</v>
@@ -6248,15 +6251,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="19">
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C111" s="39" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D111" s="19" t="s">
         <v>28</v>
@@ -6281,15 +6284,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="19">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C112" s="39" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D112" s="19" t="s">
         <v>28</v>
@@ -6314,15 +6317,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="19">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>28</v>
@@ -6347,15 +6350,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="19">
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>28</v>
@@ -6380,15 +6383,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="19">
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D115" s="19" t="s">
         <v>28</v>
@@ -6413,15 +6416,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="19">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C116" s="39" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>28</v>
@@ -6446,15 +6449,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="19">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C117" s="39" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>28</v>
@@ -6479,15 +6482,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="19">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C118" s="39" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>28</v>
@@ -6512,15 +6515,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="19">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C119" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D119" s="19" t="s">
         <v>28</v>
@@ -6544,15 +6547,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="19">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C120" s="39" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D120" s="19" t="s">
         <v>28</v>
@@ -6576,15 +6579,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="19">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C121" s="39" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D121" s="19" t="s">
         <v>28</v>
@@ -6608,15 +6611,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="19">
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C122" s="39" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D122" s="19" t="s">
         <v>28</v>
@@ -6640,15 +6643,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="19">
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C123" s="39" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D123" s="19" t="s">
         <v>28</v>
@@ -6672,15 +6675,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="19">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C124" s="39" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D124" s="19" t="s">
         <v>28</v>
@@ -6704,15 +6707,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="19">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C125" s="39" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D125" s="19" t="s">
         <v>28</v>
@@ -6736,15 +6739,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="19">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C126" s="39" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D126" s="19" t="s">
         <v>28</v>
@@ -6768,15 +6771,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="19">
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C127" s="39" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D127" s="19" t="s">
         <v>28</v>
@@ -6800,15 +6803,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="19">
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C128" s="39" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D128" s="19" t="s">
         <v>28</v>
@@ -6832,15 +6835,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="19">
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C129" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D129" s="19" t="s">
         <v>17</v>
@@ -6849,16 +6852,16 @@
         <v>11</v>
       </c>
       <c r="F129" s="46" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H129">
         <v>5</v>
       </c>
       <c r="I129" s="19" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J129" s="41" t="s">
         <v>13</v>
@@ -7166,8 +7169,8 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>

<commit_message>
KORA-5 changing order of vocational training: other to different position in hierarchy
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF50BEC-D7F2-45CB-98E5-544213FDB7A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C55481-6B10-4234-B292-21B2A70F316F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1472,21 +1472,20 @@
     <t>case_when</t>
   </si>
   <si>
+    <t>proximate</t>
+  </si>
+  <si>
     <t>case_when(
   AI13ABSC %in% c(4) | AI14ABSC %in% c(0) ~ 7L,
   AI14ABSC %in% c(3,4) ~ 6L,
   AI14ABSC %in% c(2) ~ 4L,
-  AI14ABSC %in% c(5) ~ 9L,
   AI13ABSC %in% c(3) ~ 3L,
   AI13ABSC %in% c(1,2) ~ 2L,
   AI13ABSC %in% c(6) &amp; AI14ABSC %in% c(1) ~ 0L,
   is.na(AI13ABSC) &amp; AI14ABSC %in% c(1) ~ 0L,
   AI13ABSC %in% c(6) &amp; is.na(AI14ABSC) ~ 0L,
-  AI13ABSC %in% c(5) ~ 9L,
+  AI14ABSC %in% c(5) | AI13ABSC %in% c(5) ~ 9L,
   TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>proximate</t>
   </si>
 </sst>
 </file>
@@ -2500,7 +2499,7 @@
   <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2676,14 +2675,14 @@
         <v>450</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="17" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6900,27 +6899,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -7161,10 +7139,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7187,20 +7197,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>